<commit_message>
Add new master file.
Add new master file.
</commit_message>
<xml_diff>
--- a/app/static/download/archivo-maestro.xlsx
+++ b/app/static/download/archivo-maestro.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zWork\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2065EF4-08A8-4B7B-AE2E-C746201EDDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA78A5C-5005-473A-87C6-85B4263D08BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29025" yWindow="4410" windowWidth="29415" windowHeight="11295" tabRatio="614" firstSheet="1" activeTab="1" xr2:uid="{A5E5D427-94B6-4149-BB79-F552E3020388}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="614" firstSheet="1" activeTab="2" xr2:uid="{A5E5D427-94B6-4149-BB79-F552E3020388}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" state="hidden" r:id="rId1"/>
-    <sheet name="extracto-mora" sheetId="3" r:id="rId2"/>
-    <sheet name="estado-cuenta" sheetId="4" r:id="rId3"/>
+    <sheet name="extracto-mora" sheetId="5" r:id="rId2"/>
+    <sheet name="estado-cuenta" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>ID Contacto</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>Tipo de extracto</t>
+  </si>
+  <si>
+    <t>extracto-mora</t>
+  </si>
+  <si>
+    <t>estado-cuenta</t>
   </si>
 </sst>
 </file>
@@ -700,28 +706,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62AA2D2-7260-4623-8A5A-249C09256DD6}">
-  <dimension ref="A1:Q3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE55271F-0B55-47CF-8770-F36793733284}">
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="19.5703125" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" customWidth="1"/>
-    <col min="16" max="16" width="21.140625" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -783,15 +777,9 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="P3" s="3"/>
+      <c r="Q2" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -799,24 +787,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A3B147A-38EE-4AA1-8E0E-DAC60802DAC6}">
-  <dimension ref="A1:Q1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7E31E9D-599A-4928-9D95-188B3402A9F0}">
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="17" customWidth="1"/>
-    <col min="15" max="15" width="14" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -867,10 +847,14 @@
       </c>
       <c r="Q1" s="6" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>